<commit_message>
add index, col to WorksheetColumn
</commit_message>
<xml_diff>
--- a/tests/test_rtm.xlsx
+++ b/tests/test_rtm.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\fdr\tests\unit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuki\projects\fdr\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE288E0-560E-47F9-A751-EB7AA4656BA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DD4AD7-064C-4064-AADE-E6C09094FD3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_worksheet" sheetId="21" r:id="rId1"/>
     <sheet name="Procedure Based Requirements" sheetId="22" r:id="rId2"/>
+    <sheet name="test_validation" sheetId="23" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Procedure Based Requirements'!$A$1:$O$1</definedName>
@@ -24,19 +25,38 @@
     <definedName name="rngRequirements" localSheetId="1">#REF!</definedName>
     <definedName name="rngRequirements">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4AB33BBD-8845-41EF-A55D-07BBCE08DB10}</author>
+  </authors>
+  <commentList>
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{4AB33BBD-8845-41EF-A55D-07BBCE08DB10}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    fail: val_cell_not_empty</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -84,13 +104,43 @@
   <si>
     <t>CTQ?
 Yes, No, N/A</t>
+  </si>
+  <si>
+    <t>PassOrFail</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>BodyIndex</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>val_cells_not_empty</t>
+  </si>
+  <si>
+    <t>greet</t>
+  </si>
+  <si>
+    <t>val_column_sort</t>
+  </si>
+  <si>
+    <t>val_column_exist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +216,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +269,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -293,7 +367,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -303,8 +377,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,11 +401,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
+    <cellStyle name="Bad" xfId="8" builtinId="27"/>
     <cellStyle name="Calculation" xfId="2" builtinId="22" hidden="1"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23" hidden="1"/>
     <cellStyle name="Explanatory Text" xfId="5" builtinId="53" hidden="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26"/>
     <cellStyle name="Input" xfId="1" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="3" builtinId="24" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,6 +427,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jonathan Chukinas" id="{BA95EFCC-E39B-4FD7-9BEE-F448F9FA0C93}" userId="a10c016a9ad732b9" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -643,21 +730,29 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="J3" dT="2019-07-29T20:42:57.38" personId="{BA95EFCC-E39B-4FD7-9BEE-F448F9FA0C93}" id="{4AB33BBD-8845-41EF-A55D-07BBCE08DB10}">
+    <text>fail: val_cell_not_empty</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="3" customWidth="1"/>
-    <col min="2" max="7" width="4.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="7" width="16.28515625" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="21.85546875" customWidth="1"/>
     <col min="9" max="9" width="61.5703125" style="4" customWidth="1"/>
     <col min="10" max="10" width="33.42578125" customWidth="1"/>
@@ -669,179 +764,241 @@
     <col min="16" max="16" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="str">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
         <f>_xlfn.CONCAT(A1, " value")</f>
         <v>ID value</v>
       </c>
-      <c r="B2" s="3" t="str">
-        <f t="shared" ref="B2:O3" si="0">_xlfn.CONCAT(B1, " value")</f>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:O2" si="0">_xlfn.CONCAT(B1, " value")</f>
         <v>Procedure Step value</v>
       </c>
-      <c r="C2" s="3" t="str">
+      <c r="C2" t="str">
         <f t="shared" si="0"/>
         <v>User Need value</v>
       </c>
-      <c r="D2" s="3" t="str">
+      <c r="D2" t="str">
         <f t="shared" si="0"/>
         <v>Design Input value</v>
       </c>
-      <c r="E2" s="3" t="str">
+      <c r="E2" t="str">
         <f t="shared" si="0"/>
         <v>DO Solution L1 value</v>
       </c>
-      <c r="F2" s="3" t="str">
+      <c r="F2" t="str">
         <f t="shared" si="0"/>
         <v>DO Solution L2 value</v>
       </c>
-      <c r="G2" s="3" t="str">
+      <c r="G2" t="str">
         <f t="shared" si="0"/>
         <v>DO Solution L3 value</v>
       </c>
-      <c r="H2" s="3" t="str">
+      <c r="H2" t="str">
         <f t="shared" si="0"/>
         <v>Cascade Level value</v>
       </c>
-      <c r="I2" s="3" t="str">
+      <c r="I2" t="str">
         <f t="shared" si="0"/>
         <v>Requirement Statement value</v>
       </c>
-      <c r="J2" s="3" t="str">
+      <c r="J2" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Requirement Rationale value</v>
       </c>
-      <c r="K2" s="3" t="str">
+      <c r="K2" t="str">
         <f t="shared" si="0"/>
         <v>Verification or
 Validation Strategy value</v>
       </c>
-      <c r="L2" s="3" t="str">
+      <c r="L2" t="str">
         <f t="shared" si="0"/>
         <v>Verification or Validation Results value</v>
       </c>
-      <c r="M2" s="3" t="str">
+      <c r="M2" t="str">
         <f t="shared" si="0"/>
         <v>Devices value</v>
       </c>
-      <c r="N2" s="3" t="str">
+      <c r="N2" t="str">
         <f t="shared" si="0"/>
         <v>Design Ouptut Feature
 (with CTQ ID #) value</v>
       </c>
-      <c r="O2" s="3" t="str">
+      <c r="O2" t="str">
         <f t="shared" si="0"/>
         <v>CTQ?
 Yes, No, N/A value</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="str">
-        <f>_xlfn.CONCAT(A2, " value")</f>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:I3" si="1">_xlfn.CONCAT(A1, " value")</f>
+        <v>ID value</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="1"/>
+        <v>Procedure Step value</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="1"/>
+        <v>User Need value</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>Design Input value</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="1"/>
+        <v>DO Solution L1 value</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="1"/>
+        <v>DO Solution L2 value</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="1"/>
+        <v>DO Solution L3 value</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="1"/>
+        <v>Cascade Level value</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="1"/>
+        <v>Requirement Statement value</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:O4" si="2">_xlfn.CONCAT(K1, " value")</f>
+        <v>Verification or
+Validation Strategy value</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="2"/>
+        <v>Verification or Validation Results value</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="2"/>
+        <v>Devices value</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" si="2"/>
+        <v>Design Ouptut Feature
+(with CTQ ID #) value</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="2"/>
+        <v>CTQ?
+Yes, No, N/A value</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:I4" si="3">_xlfn.CONCAT(A2, " value")</f>
         <v>ID value value</v>
       </c>
-      <c r="B3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="B4" t="str">
+        <f t="shared" si="3"/>
         <v>Procedure Step value value</v>
       </c>
-      <c r="C3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="C4" t="str">
+        <f t="shared" si="3"/>
         <v>User Need value value</v>
       </c>
-      <c r="D3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="D4" t="str">
+        <f t="shared" si="3"/>
         <v>Design Input value value</v>
       </c>
-      <c r="E3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="E4" t="str">
+        <f t="shared" si="3"/>
         <v>DO Solution L1 value value</v>
       </c>
-      <c r="F3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="F4" t="str">
+        <f t="shared" si="3"/>
         <v>DO Solution L2 value value</v>
       </c>
-      <c r="G3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="G4" t="str">
+        <f t="shared" si="3"/>
         <v>DO Solution L3 value value</v>
       </c>
-      <c r="H3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
         <v>Cascade Level value value</v>
       </c>
-      <c r="I3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="I4" t="str">
+        <f t="shared" si="3"/>
         <v>Requirement Statement value value</v>
       </c>
-      <c r="J3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="J4" s="8" t="str">
+        <f>_xlfn.CONCAT(J2, " value")</f>
         <v>Requirement Rationale value value</v>
       </c>
-      <c r="K3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="K4" t="str">
+        <f t="shared" si="2"/>
         <v>Verification or
 Validation Strategy value value</v>
       </c>
-      <c r="L3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
         <v>Verification or Validation Results value value</v>
       </c>
-      <c r="M3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="M4" t="str">
+        <f t="shared" si="2"/>
         <v>Devices value value</v>
       </c>
-      <c r="N3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="N4" t="str">
+        <f t="shared" si="2"/>
         <v>Design Ouptut Feature
 (with CTQ ID #) value value</v>
       </c>
-      <c r="O3" s="3" t="str">
-        <f t="shared" si="0"/>
+      <c r="O4" t="str">
+        <f t="shared" si="2"/>
         <v>CTQ?
 Yes, No, N/A value value</v>
       </c>
@@ -853,6 +1010,7 @@
   <headerFooter>
     <oddFooter>&amp;CPage &amp;P of &amp;N&amp;RVersion 2.0</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1069,7 +1227,192 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F75445-3309-40FF-A033-8608838D7335}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Deliverable xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <Workstream xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <Project xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <OpCo xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45">DPS Trauma</OpCo>
+    <SharedWithUsers xmlns="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b">
+      <UserInfo>
+        <DisplayName>Dec, Brian [SYNNA]</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Conley, Jordan [SYNNA]</DisplayName>
+        <AccountId>6</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Tarczewski, John [DPYUS NON-J&amp;J]</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Valenzuela, Jan [DPYUS]</DisplayName>
+        <AccountId>34</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <Archive xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45">false</Archive>
+    <MovetoWorkstream_x003f_ xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1078,7 +1421,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B2369C55104614D86A5ED6959977478" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0e7eb4f9a047313f41567777b26d1b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e53f4f12-70f6-49ff-8342-256ad4d5af45" xmlns:ns3="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="21513b83e70fc08b789b5f083b414370" ns2:_="" ns3:_="">
     <xsd:import namespace="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
@@ -1357,42 +1700,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Deliverable xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <Workstream xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <Project xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <OpCo xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45">DPS Trauma</OpCo>
-    <SharedWithUsers xmlns="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b">
-      <UserInfo>
-        <DisplayName>Dec, Brian [SYNNA]</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Conley, Jordan [SYNNA]</DisplayName>
-        <AccountId>6</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Tarczewski, John [DPYUS NON-J&amp;J]</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Valenzuela, Jan [DPYUS]</DisplayName>
-        <AccountId>34</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <Archive xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45">false</Archive>
-    <MovetoWorkstream_x003f_ xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6B224B-0E2C-48D8-BDA5-831DA84116C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EA3E94-102E-42ED-8307-567DE6417681}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1400,7 +1725,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB17CD09-13F0-4BBC-ACF0-5247DAC323D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1417,21 +1742,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6B224B-0E2C-48D8-BDA5-831DA84116C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
markup, subdir, open & version check
replace pypi-get with requests

version markup works

done

fix field not found message

add convert header to string

file now opens after markup

markup, subdir, open & version check

v25 -> v26
</commit_message>
<xml_diff>
--- a/tests/test_rtm.xlsx
+++ b/tests/test_rtm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\rtm\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6551465-603A-437C-920F-8BB2BC982D9B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B976C7-04BB-48F3-8215-AEF64A100675}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1592,7 +1592,7 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1709,9 +1709,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -2328,9 +2325,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O80"/>
+  <dimension ref="A2:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2347,9 +2346,6 @@
     <col min="16" max="16" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43"/>
-    </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
add id header to test worksheet
</commit_message>
<xml_diff>
--- a/tests/test_rtm.xlsx
+++ b/tests/test_rtm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\rtm\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6551465-603A-437C-920F-8BB2BC982D9B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D9BF3D-9E45-4FA2-B5C3-9F8DF71B9146}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_worksheet" sheetId="21" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="328">
   <si>
     <t>ID</t>
   </si>
@@ -1258,6 +1258,9 @@
 Crest length
 Overall length</t>
     </r>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -2054,7 +2057,7 @@
   </sheetPr>
   <dimension ref="A2:O5"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -2330,7 +2333,9 @@
   </sheetPr>
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2350,8 +2355,8 @@
     <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43"/>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -5354,145 +5359,148 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F75445-3309-40FF-A033-8608838D7335}">
-  <dimension ref="A2:E12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>A3+1</f>
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f>B2+1</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="str">
+      <c r="D3" t="str">
         <f>""</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" ref="A5:A12" si="0">A4+1</f>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f t="shared" ref="B4:B11" si="0">B3+1</f>
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
+      <c r="D7">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="C11">
+      <c r="D10">
         <f>2*4</f>
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5504,67 +5512,70 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E10630-D1E9-46DB-98CF-4A34D3F758E6}">
-  <dimension ref="A2:D5"/>
+  <dimension ref="B3:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="C6">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="E6">
         <v>3</v>
       </c>
     </row>
@@ -5575,126 +5586,126 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34283C52-A606-4A91-BE38-3A1E2EFABC11}">
-  <dimension ref="A2:AA27"/>
+  <dimension ref="A2:AB27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" style="1" customWidth="1"/>
-    <col min="14" max="19" width="4.7109375" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="25" customWidth="1"/>
-    <col min="22" max="22" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1"/>
-    <col min="25" max="25" width="12" customWidth="1"/>
-    <col min="26" max="26" width="8.5703125" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" style="1" customWidth="1"/>
+    <col min="15" max="20" width="4.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="25" customWidth="1"/>
+    <col min="23" max="23" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" customWidth="1"/>
+    <col min="26" max="26" width="12" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" s="4" customFormat="1" ht="148.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" s="4" customFormat="1" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>1</v>
-      </c>
       <c r="O2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="AA2" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AB2" s="13" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>-1</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
@@ -5704,7 +5715,7 @@
       <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="1" t="b">
+      <c r="H3" t="b">
         <v>1</v>
       </c>
       <c r="J3" s="1" t="b">
@@ -5713,60 +5724,60 @@
       <c r="K3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>39</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>310</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>295</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="Z3" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="Z3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>A3+1</f>
-        <v>1</v>
-      </c>
+      <c r="AA3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>B3+1</f>
         <v>1</v>
       </c>
       <c r="C4">
-        <f>A3</f>
+        <f>C3+1</f>
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f>B3</f>
         <v>0</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
       <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
       <c r="G4" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="1" t="b">
+      <c r="H4" t="b">
         <v>1</v>
       </c>
       <c r="J4" s="1" t="b">
@@ -5775,54 +5786,54 @@
       <c r="K4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="N4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>40</v>
       </c>
-      <c r="V4" s="14" t="s">
+      <c r="W4" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>303</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>302</v>
       </c>
-      <c r="Z4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" ref="A5:B27" si="0">A4+1</f>
+      <c r="AA4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" ref="B5:C27" si="0">B4+1</f>
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C5">
-        <f t="shared" ref="C5:C8" si="1">A4</f>
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
+      <c r="D5">
+        <f t="shared" ref="D5:D8" si="1">B4</f>
         <v>1</v>
       </c>
       <c r="E5" t="b">
@@ -5834,7 +5845,7 @@
       <c r="G5" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="1" t="b">
+      <c r="H5" t="b">
         <v>1</v>
       </c>
       <c r="J5" s="1" t="b">
@@ -5843,47 +5854,47 @@
       <c r="K5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1" t="s">
+      <c r="N5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="14" t="s">
+      <c r="W5" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>304</v>
       </c>
-      <c r="Z5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="AA5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
@@ -5893,56 +5904,56 @@
       <c r="G6" t="b">
         <v>1</v>
       </c>
-      <c r="I6" s="1" t="b">
+      <c r="H6" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="L6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
         <v>52</v>
       </c>
-      <c r="M6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1" t="s">
+      <c r="N6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>45</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="W6" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>305</v>
       </c>
-      <c r="Z6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA6" t="b">
+      <c r="AA6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
@@ -5952,7 +5963,7 @@
       <c r="G7" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="1" t="b">
+      <c r="H7" t="b">
         <v>1</v>
       </c>
       <c r="J7" s="1" t="b">
@@ -5961,57 +5972,57 @@
       <c r="K7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
         <v>53</v>
       </c>
-      <c r="M7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="R7" s="1" t="s">
+      <c r="N7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>101</v>
       </c>
-      <c r="V7" s="14" t="s">
+      <c r="W7" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>311</v>
       </c>
-      <c r="Z7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+      <c r="AA7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
         <v>0</v>
       </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="b">
+      <c r="H8" t="b">
         <v>1</v>
       </c>
       <c r="J8" s="1" t="b">
@@ -6020,44 +6031,44 @@
       <c r="K8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="S8" s="1" t="s">
+      <c r="N8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>101</v>
       </c>
-      <c r="V8" s="14" t="s">
+      <c r="W8" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="Z8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="AA8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9">
-        <f>B8</f>
+      <c r="C9">
+        <f>C8</f>
         <v>5</v>
       </c>
-      <c r="C9">
-        <f>A7</f>
+      <c r="D9">
+        <f>B7</f>
         <v>4</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
@@ -6065,53 +6076,53 @@
         <v>1</v>
       </c>
       <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>55</v>
       </c>
-      <c r="M9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="S9" s="1" t="s">
+      <c r="N9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>39</v>
       </c>
-      <c r="V9" s="14"/>
-      <c r="Z9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="W9" s="14"/>
+      <c r="AA9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10">
-        <f>B7</f>
-        <v>4</v>
-      </c>
       <c r="C10">
         <f>C7</f>
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f>D7</f>
         <v>3</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
@@ -6121,52 +6132,52 @@
       <c r="G10" t="b">
         <v>1</v>
       </c>
-      <c r="I10" s="1" t="b">
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
         <v>56</v>
       </c>
-      <c r="M10" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="R10" s="1" t="s">
+      <c r="N10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z10" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="AA10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>-1</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
       </c>
-      <c r="I11" s="1" t="b">
+      <c r="H11" t="b">
         <v>1</v>
       </c>
       <c r="J11" s="1" t="b">
@@ -6175,37 +6186,37 @@
       <c r="K11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="U11" t="s">
+      <c r="N11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="V11" t="s">
         <v>101</v>
       </c>
-      <c r="Z11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="AA11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>3</v>
       </c>
-      <c r="C12">
-        <f>C6</f>
+      <c r="D12">
+        <f>D6</f>
         <v>2</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
       <c r="E12" t="b">
         <v>1</v>
       </c>
@@ -6215,47 +6226,47 @@
       <c r="G12" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="1" t="b">
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J12" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="1" t="s">
+      <c r="N12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>298</v>
       </c>
-      <c r="Z12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="AA12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B13">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>2</v>
       </c>
-      <c r="C13">
-        <f>C5</f>
-        <v>1</v>
-      </c>
-      <c r="D13" t="b">
+      <c r="D13">
+        <f>D5</f>
         <v>1</v>
       </c>
       <c r="E13" t="b">
@@ -6267,48 +6278,48 @@
       <c r="G13" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="1" t="b">
+      <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="J13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>59</v>
       </c>
-      <c r="M13" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="P13" s="1" t="s">
+      <c r="N13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>39</v>
       </c>
-      <c r="Z13" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="AA13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B14">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>-1</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
@@ -6318,48 +6329,48 @@
       <c r="G14" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="1" t="b">
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J14" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="1" t="s">
+      <c r="N14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V14" s="14" t="s">
+      <c r="W14" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="Z14" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="AA14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>3</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>-1</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
       <c r="E15" t="b">
         <v>1</v>
       </c>
@@ -6369,48 +6380,48 @@
       <c r="G15" t="b">
         <v>1</v>
       </c>
-      <c r="I15" s="1" t="b">
+      <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="J15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>60</v>
       </c>
-      <c r="M15" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="1" t="s">
+      <c r="N15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>39</v>
       </c>
-      <c r="Z15" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="AA15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B16">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>2</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>-1</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
       <c r="E16" t="b">
         <v>1</v>
       </c>
@@ -6420,48 +6431,48 @@
       <c r="G16" t="b">
         <v>1</v>
       </c>
-      <c r="I16" s="1" t="b">
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J16" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
         <v>61</v>
       </c>
-      <c r="M16" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="P16" s="1" t="s">
+      <c r="N16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>300</v>
       </c>
-      <c r="Z16" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="AA16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>4</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>-1</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
       <c r="E17" t="b">
         <v>1</v>
       </c>
@@ -6471,48 +6482,48 @@
       <c r="G17" t="b">
         <v>1</v>
       </c>
-      <c r="I17" s="1" t="b">
+      <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="J17" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>62</v>
       </c>
-      <c r="M17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="R17" s="1" t="s">
+      <c r="N17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>39</v>
       </c>
-      <c r="Z17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="AA17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B18">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="12">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12">
         <v>11</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
       <c r="E18" t="b">
         <v>1</v>
       </c>
@@ -6522,7 +6533,7 @@
       <c r="G18" t="b">
         <v>1</v>
       </c>
-      <c r="I18" s="1" t="b">
+      <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="J18" s="1" t="b">
@@ -6531,84 +6542,84 @@
       <c r="K18" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
         <v>63</v>
       </c>
-      <c r="M18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O18" s="1" t="s">
+      <c r="N18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>87</v>
       </c>
-      <c r="Z18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="AA18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B19">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>-1</v>
-      </c>
-      <c r="D19" t="b">
-        <v>0</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
       </c>
-      <c r="I19" s="1" t="b">
+      <c r="H19" t="b">
         <v>1</v>
       </c>
       <c r="J19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="L19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
         <v>64</v>
       </c>
-      <c r="M19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="U19" t="s">
+      <c r="N19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="V19" t="s">
         <v>45</v>
       </c>
-      <c r="Z19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="AA19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B20">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>15</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
       <c r="E20" t="b">
         <v>1</v>
       </c>
@@ -6618,156 +6629,156 @@
       <c r="G20" t="b">
         <v>1</v>
       </c>
-      <c r="I20" s="1" t="b">
+      <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="J20" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>65</v>
       </c>
-      <c r="M20" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="P20" s="1" t="s">
+      <c r="N20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>101</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>315</v>
       </c>
-      <c r="Z20" s="1" t="b">
+      <c r="AA20" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="AA20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="AB20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B21">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>2</v>
       </c>
-      <c r="C21">
-        <f>C20</f>
+      <c r="D21">
+        <f>D20</f>
         <v>15</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
       <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
         <v>0</v>
       </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
       <c r="G21" t="b">
         <v>1</v>
       </c>
-      <c r="I21" s="1" t="b">
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J21" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K21" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" t="s">
         <v>66</v>
       </c>
-      <c r="M21" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>25</v>
+      <c r="N21" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V21" t="s">
+      <c r="R21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W21" t="s">
         <v>316</v>
       </c>
-      <c r="Z21" s="1" t="b">
+      <c r="AA21" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="AA21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="AB21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B22">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>3</v>
       </c>
-      <c r="C22">
-        <f>A21</f>
+      <c r="D22">
+        <f>B21</f>
         <v>18</v>
       </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
       <c r="E22" t="b">
         <v>1</v>
       </c>
       <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
         <v>0</v>
       </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1" t="b">
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J22" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K22" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
         <v>67</v>
       </c>
-      <c r="M22" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="1" t="s">
+      <c r="N22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z22" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="AA22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B23">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
       <c r="C23">
-        <f>C18</f>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f>D18</f>
         <v>11</v>
       </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
       <c r="E23" t="b">
         <v>1</v>
       </c>
@@ -6777,7 +6788,7 @@
       <c r="G23" t="b">
         <v>1</v>
       </c>
-      <c r="I23" s="1" t="b">
+      <c r="H23" t="b">
         <v>1</v>
       </c>
       <c r="J23" s="1" t="b">
@@ -6786,40 +6797,40 @@
       <c r="K23" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" t="s">
         <v>68</v>
       </c>
-      <c r="M23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O23" s="1" t="s">
+      <c r="N23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>41</v>
       </c>
-      <c r="Z23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="AA23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B24">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>2</v>
       </c>
-      <c r="C24">
-        <f>A23</f>
+      <c r="D24">
+        <f>B23</f>
         <v>20</v>
       </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
       <c r="E24" t="b">
         <v>1</v>
       </c>
@@ -6827,48 +6838,48 @@
         <v>1</v>
       </c>
       <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="1" t="b">
+      <c r="J24" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J24" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K24" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
         <v>69</v>
       </c>
-      <c r="M24" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="P24" s="1" t="s">
+      <c r="N24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Z24" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="AA24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B25">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>3</v>
       </c>
-      <c r="C25">
-        <f t="shared" ref="C25:C27" si="2">A24</f>
+      <c r="D25">
+        <f t="shared" ref="D25:D27" si="2">B24</f>
         <v>21</v>
       </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
       <c r="E25" t="b">
         <v>1</v>
       </c>
@@ -6878,46 +6889,46 @@
       <c r="G25" t="b">
         <v>1</v>
       </c>
-      <c r="I25" s="1" t="b">
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J25" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K25" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25" t="s">
         <v>70</v>
       </c>
-      <c r="M25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="1" t="s">
+      <c r="N25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="AA25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B26">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>4</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
       <c r="E26" t="b">
         <v>1</v>
       </c>
@@ -6927,85 +6938,88 @@
       <c r="G26" t="b">
         <v>1</v>
       </c>
-      <c r="I26" s="1" t="b">
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J26" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K26" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
         <v>71</v>
       </c>
-      <c r="M26" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="R26" s="1" t="s">
+      <c r="N26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>317</v>
       </c>
-      <c r="Z26" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA26" t="b">
+      <c r="AA26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B27">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>5</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
       <c r="E27" t="b">
         <v>1</v>
       </c>
       <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" t="b">
         <v>0</v>
       </c>
-      <c r="G27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="1" t="b">
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J27" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K27" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
         <v>72</v>
       </c>
-      <c r="M27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="S27" s="1" t="s">
+      <c r="N27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="T27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA27" t="b">
+      <c r="AA27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB27" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I3:K27">
+  <conditionalFormatting sqref="J3:L27">
     <cfRule type="iconSet" priority="3">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -7024,7 +7038,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:Z27">
+  <conditionalFormatting sqref="AA3:AA27">
     <cfRule type="iconSet" priority="1">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -7050,10 +7064,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10D0E2C-1B2C-4DA2-B0A4-E7A32A693220}">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7062,15 +7076,18 @@
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>289</v>
       </c>
       <c r="B2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -7078,7 +7095,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+1</f>
         <v>1</v>
@@ -7087,7 +7104,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5" si="0">A4+1</f>
         <v>2</v>
@@ -7111,6 +7128,26 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Deliverable xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <Workstream xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <Project xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <OpCo xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <SharedWithUsers xmlns="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <Archive xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <MovetoWorkstream_x003f_ xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B2369C55104614D86A5ED6959977478" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0e7eb4f9a047313f41567777b26d1b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e53f4f12-70f6-49ff-8342-256ad4d5af45" xmlns:ns3="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="21513b83e70fc08b789b5f083b414370" ns2:_="" ns3:_="">
     <xsd:import namespace="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
@@ -7389,26 +7426,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Deliverable xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <Workstream xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <Project xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <OpCo xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <SharedWithUsers xmlns="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <Archive xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <MovetoWorkstream_x003f_ xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EA3E94-102E-42ED-8307-567DE6417681}">
   <ds:schemaRefs>
@@ -7418,6 +7435,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6B224B-0E2C-48D8-BDA5-831DA84116C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b"/>
+    <ds:schemaRef ds:uri="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB17CD09-13F0-4BBC-ACF0-5247DAC323D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7434,21 +7468,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6B224B-0E2C-48D8-BDA5-831DA84116C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b"/>
-    <ds:schemaRef ds:uri="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
trying to fix test_validation
</commit_message>
<xml_diff>
--- a/tests/test_rtm.xlsx
+++ b/tests/test_rtm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\rtm\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D9BF3D-9E45-4FA2-B5C3-9F8DF71B9146}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6062301-B89F-4F22-8EEA-6252C59170D2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_worksheet" sheetId="21" r:id="rId1"/>
@@ -2057,7 +2057,7 @@
   </sheetPr>
   <dimension ref="A2:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -5514,8 +5514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E10630-D1E9-46DB-98CF-4A34D3F758E6}">
   <dimension ref="B3:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5550,6 +5550,9 @@
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -5564,6 +5567,9 @@
       <c r="E5">
         <v>2</v>
       </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -5576,6 +5582,9 @@
         <v>3</v>
       </c>
       <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
         <v>3</v>
       </c>
     </row>
@@ -7119,35 +7128,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Deliverable xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <Workstream xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <Project xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <OpCo xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <SharedWithUsers xmlns="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <Archive xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <MovetoWorkstream_x003f_ xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B2369C55104614D86A5ED6959977478" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0e7eb4f9a047313f41567777b26d1b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e53f4f12-70f6-49ff-8342-256ad4d5af45" xmlns:ns3="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="21513b83e70fc08b789b5f083b414370" ns2:_="" ns3:_="">
     <xsd:import namespace="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
@@ -7426,10 +7406,50 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Deliverable xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <Workstream xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <Project xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <OpCo xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <SharedWithUsers xmlns="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <Archive xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <MovetoWorkstream_x003f_ xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EA3E94-102E-42ED-8307-567DE6417681}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB17CD09-13F0-4BBC-ACF0-5247DAC323D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
+    <ds:schemaRef ds:uri="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7452,20 +7472,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB17CD09-13F0-4BBC-ACF0-5247DAC323D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EA3E94-102E-42ED-8307-567DE6417681}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
-    <ds:schemaRef ds:uri="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
functions for finding string best matches
</commit_message>
<xml_diff>
--- a/tests/test_rtm.xlsx
+++ b/tests/test_rtm.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\rtm\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B976C7-04BB-48F3-8215-AEF64A100675}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D19E0A-F036-46D1-8020-B83D0A1D12D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_worksheet" sheetId="21" r:id="rId1"/>
     <sheet name="Procedure Based Requirements" sheetId="27" r:id="rId2"/>
-    <sheet name="Procedure Based Requirements2" sheetId="22" r:id="rId3"/>
-    <sheet name="test_validation" sheetId="23" r:id="rId4"/>
-    <sheet name="nonsense_fields" sheetId="26" r:id="rId5"/>
-    <sheet name="cascade" sheetId="25" r:id="rId6"/>
-    <sheet name="tags" sheetId="28" r:id="rId7"/>
+    <sheet name="pandas_experiment" sheetId="29" r:id="rId3"/>
+    <sheet name="Procedure Based Requirements2" sheetId="22" r:id="rId4"/>
+    <sheet name="test_validation" sheetId="23" r:id="rId5"/>
+    <sheet name="nonsense_fields" sheetId="26" r:id="rId6"/>
+    <sheet name="cascade" sheetId="25" r:id="rId7"/>
+    <sheet name="tags" sheetId="28" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Procedure Based Requirements'!$A$2:$O$80</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Procedure Based Requirements2'!$A$2:$O$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Procedure Based Requirements2'!$A$2:$O$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_worksheet!$A$2:$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="338">
   <si>
     <t>ID</t>
   </si>
@@ -1258,6 +1259,39 @@
 Crest length
 Overall length</t>
     </r>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>bye</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>bye1</t>
+  </si>
+  <si>
+    <t>bye2</t>
+  </si>
+  <si>
+    <t>bye3</t>
+  </si>
+  <si>
+    <t>bye14</t>
+  </si>
+  <si>
+    <t>bye15</t>
+  </si>
+  <si>
+    <t>bye16</t>
   </si>
 </sst>
 </file>
@@ -2327,7 +2361,7 @@
   </sheetPr>
   <dimension ref="A2:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -5125,6 +5159,77 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5130B73-D7FF-4016-BA55-6FA2C744F3EA}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B51914-4951-4CB5-B02A-D6D464BC6724}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -5348,7 +5453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F75445-3309-40FF-A033-8608838D7335}">
   <dimension ref="A2:E12"/>
   <sheetViews>
@@ -5498,7 +5603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E10630-D1E9-46DB-98CF-4A34D3F758E6}">
   <dimension ref="A2:D5"/>
   <sheetViews>
@@ -5569,7 +5674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34283C52-A606-4A91-BE38-3A1E2EFABC11}">
   <dimension ref="A2:AA27"/>
   <sheetViews>
@@ -7044,7 +7149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10D0E2C-1B2C-4DA2-B0A4-E7A32A693220}">
   <dimension ref="A2:B5"/>
   <sheetViews>

</xml_diff>

<commit_message>
successfully reading dataframe while seeking header row
</commit_message>
<xml_diff>
--- a/tests/test_rtm.xlsx
+++ b/tests/test_rtm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\rtm\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D19E0A-F036-46D1-8020-B83D0A1D12D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7250D4-C218-48F0-BBEC-1517A2EA3E9A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_worksheet" sheetId="21" r:id="rId1"/>
@@ -1261,9 +1261,6 @@
     </r>
   </si>
   <si>
-    <t>good</t>
-  </si>
-  <si>
     <t>bye</t>
   </si>
   <si>
@@ -1276,22 +1273,25 @@
     <t>c</t>
   </si>
   <si>
-    <t>bye1</t>
-  </si>
-  <si>
-    <t>bye2</t>
-  </si>
-  <si>
-    <t>bye3</t>
-  </si>
-  <si>
-    <t>bye14</t>
-  </si>
-  <si>
-    <t>bye15</t>
-  </si>
-  <si>
-    <t>bye16</t>
+    <t>fdsa</t>
+  </si>
+  <si>
+    <t>fsda</t>
+  </si>
+  <si>
+    <t>fds</t>
+  </si>
+  <si>
+    <t>jona</t>
+  </si>
+  <si>
+    <t>nic</t>
+  </si>
+  <si>
+    <t>kri</t>
+  </si>
+  <si>
+    <t>sappy</t>
   </si>
 </sst>
 </file>
@@ -5160,68 +5160,68 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5130B73-D7FF-4016-BA55-6FA2C744F3EA}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="B3:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E3" t="s">
         <v>327</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>328</v>
       </c>
-      <c r="D1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E5" t="s">
+        <v>331</v>
+      </c>
+      <c r="F5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>329</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E6" t="s">
+        <v>335</v>
+      </c>
+      <c r="F6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E7" t="s">
+        <v>336</v>
+      </c>
+      <c r="F7" t="s">
         <v>332</v>
-      </c>
-      <c r="D2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>330</v>
-      </c>
-      <c r="C3" t="s">
-        <v>333</v>
-      </c>
-      <c r="D3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C4" t="s">
-        <v>334</v>
-      </c>
-      <c r="D4" t="s">
-        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -7212,6 +7212,26 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Deliverable xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <Workstream xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <Project xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <OpCo xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <SharedWithUsers xmlns="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <Archive xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+    <MovetoWorkstream_x003f_ xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004B2369C55104614D86A5ED6959977478" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c0e7eb4f9a047313f41567777b26d1b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e53f4f12-70f6-49ff-8342-256ad4d5af45" xmlns:ns3="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="21513b83e70fc08b789b5f083b414370" ns2:_="" ns3:_="">
     <xsd:import namespace="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
@@ -7490,26 +7510,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Deliverable xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <Workstream xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <Project xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <OpCo xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <SharedWithUsers xmlns="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <Archive xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-    <MovetoWorkstream_x003f_ xmlns="e53f4f12-70f6-49ff-8342-256ad4d5af45" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EA3E94-102E-42ED-8307-567DE6417681}">
   <ds:schemaRefs>
@@ -7519,6 +7519,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6B224B-0E2C-48D8-BDA5-831DA84116C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b"/>
+    <ds:schemaRef ds:uri="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB17CD09-13F0-4BBC-ACF0-5247DAC323D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7535,21 +7552,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6B224B-0E2C-48D8-BDA5-831DA84116C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4f4d318f-1e15-433d-b7fd-4a4fd8f11b5b"/>
-    <ds:schemaRef ds:uri="e53f4f12-70f6-49ff-8342-256ad4d5af45"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>